<commit_message>
equals-space-missing-validator All functionality has been completed and the tests have been carried out. There is now a test folder containing files to use for tests.
</commit_message>
<xml_diff>
--- a/Testing/Tests.xlsx
+++ b/Testing/Tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://appriver3651000674-my.sharepoint.com/personal/christa_pebblepad_co_uk/Documents/Documents/Uni/Year 1/Semester 1/Introduction to Programming and Problem Solving/Final Project/code-style-checker/Testing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="374" documentId="8_{146811CC-DAA1-4F5D-80B1-AA29152A21C1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{AC79B6FA-E111-49A8-8E12-1AD306E5FB94}"/>
+  <xr:revisionPtr revIDLastSave="434" documentId="8_{146811CC-DAA1-4F5D-80B1-AA29152A21C1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{BBE63439-B433-4D3D-AAF2-8A0CA592B684}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{A17C4D5C-29D9-4B29-B0BC-9381D336A1F9}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="43">
   <si>
     <t>Test</t>
   </si>
@@ -106,6 +106,63 @@
   </si>
   <si>
     <t>Delete the previously inputted text and click elsewhere on the interface.</t>
+  </si>
+  <si>
+    <t>equals-space-missing-validator</t>
+  </si>
+  <si>
+    <t>Copy the contents of ESMPass.js into the input box and press the validate button.</t>
+  </si>
+  <si>
+    <t>Copy the contents of ESMFail1.js into the input box and press the validate button.</t>
+  </si>
+  <si>
+    <t>Copy the contents of ESMFail2.js into the input box and press the validate button.</t>
+  </si>
+  <si>
+    <t>Copy the contents of ESMFail3.js into the input box and press the validate button.</t>
+  </si>
+  <si>
+    <t>Copy the contents of ESMFail4.js into the input box and press the validate button.</t>
+  </si>
+  <si>
+    <t>Copy the contents of ESMFail5.js into the input box and press the validate button.</t>
+  </si>
+  <si>
+    <t>The output box should be green and display "There are no style errors in the code!"</t>
+  </si>
+  <si>
+    <t>The output box should be red and display "There are 2 style errors in the code". The two errors should indicate that a space is needed on the left and right on the equals signs on line 3 and 4.</t>
+  </si>
+  <si>
+    <t>The output box should be red and display "There are 4 style errors in the code". The two errors should indicate that a space is needed on the left and right on the two equals signs on line 3.</t>
+  </si>
+  <si>
+    <t>The output box should be red and display "There are 2 style errors in the code". The two errors should indicate that a space is needed on the left and right on the equals sign on line 3.</t>
+  </si>
+  <si>
+    <t>The output box was green and displayed "There are no style errors in the code!"</t>
+  </si>
+  <si>
+    <t>The output box was red and displayed "There are 2 style errors in the code". The two errors indicated that a space is needed on the left and right on the equals sign on line 3.</t>
+  </si>
+  <si>
+    <t>The output box was red and displayed "There are 4 style errors in the code". The two errors indicated that a space is needed on the left and right on the two equals signs on line 3.</t>
+  </si>
+  <si>
+    <t>The output box should be red and display "There are 4 style errors in the code". The two errors should indicate that a space is needed on the left and right on the equals signs on lines 3 and 4.</t>
+  </si>
+  <si>
+    <t>The output box was red and displayed "There are 4 style errors in the code". The two errors indicated that a space is needed on the left and right on the equals signs on lines 3 and 4.</t>
+  </si>
+  <si>
+    <t>The output box was red and displayed "There are 2 style errors in the code". The two errors indicated that a space is needed on the left and right on the equals signs on line 3 and 4.</t>
+  </si>
+  <si>
+    <t>The output box should be red and display "There is 1 style error in the code". The error will indicate that a space is needed on the right of the equals sign on line 3.</t>
+  </si>
+  <si>
+    <t>The output box was red and displayed "There is 1 style error in the code". The error will indicate that a space is needed on the right of the equals sign on line 3.</t>
   </si>
 </sst>
 </file>
@@ -157,7 +214,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -180,169 +237,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -353,44 +253,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -709,8 +594,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1646CE4-CED7-43C5-9C51-B4767B3743F1}">
   <dimension ref="A1:D245"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -725,188 +610,258 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="9" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="13"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="15"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D7" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="D8" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A9" s="16" t="s">
+      <c r="A9" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="9" t="s">
+      <c r="D9" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="9" t="s">
+      <c r="D10" s="7" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="10" t="s">
+    <row r="11" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A11" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="12" t="s">
+      <c r="D11" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A12" s="2"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A13" s="2"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A14" s="2"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A15" s="2"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A16" s="2"/>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A17" s="2"/>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A18" s="2"/>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A12" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+    </row>
+    <row r="13" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+      <c r="A13" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+      <c r="A14" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+      <c r="A15" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+      <c r="A16" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+      <c r="A17" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+      <c r="A18" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" s="2"/>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" s="2"/>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="2"/>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" s="2"/>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" s="2"/>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" s="2"/>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" s="2"/>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" s="2"/>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" s="2"/>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" s="2"/>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" s="2"/>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" s="2"/>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" s="2"/>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" s="2"/>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.35">
@@ -1549,8 +1504,9 @@
       <c r="A245" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A4:D4"/>
+    <mergeCell ref="A12:D12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>